<commit_message>
add vba of Date Sort
</commit_message>
<xml_diff>
--- a/Intro.xlsx
+++ b/Intro.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sketch" sheetId="1" r:id="rId1"/>
     <sheet name="data" sheetId="2" r:id="rId2"/>
     <sheet name="edge_df" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data!$A$1:$L$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data!$A$1:$L$14</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -257,6 +257,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1730,6 +1734,77 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>31750</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>14</xdr:col>
+          <xdr:colOff>387350</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>95250</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2049" name="Button 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="54864" rIns="36576" bIns="54864" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="游ゴシック"/>
+                  <a:ea typeface="游ゴシック"/>
+                </a:rPr>
+                <a:t>Date ASC</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -1993,6 +2068,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2076,13 +2152,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -2171,7 +2245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -2185,7 +2259,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E15" si="0">1-D3</f>
+        <f>1-D3</f>
         <v>0</v>
       </c>
       <c r="F3">
@@ -2210,7 +2284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2224,7 +2298,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="0"/>
+        <f>1-D4</f>
         <v>1</v>
       </c>
       <c r="F4">
@@ -2249,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2263,7 +2337,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="0"/>
+        <f>1-D5</f>
         <v>1</v>
       </c>
       <c r="F5">
@@ -2288,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -2302,7 +2376,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
+        <f>1-D6</f>
         <v>0</v>
       </c>
       <c r="F6">
@@ -2327,7 +2401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2341,7 +2415,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
+        <f>1-D7</f>
         <v>0</v>
       </c>
       <c r="F7">
@@ -2380,7 +2454,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
+        <f>1-D8</f>
         <v>0</v>
       </c>
       <c r="F8">
@@ -2405,7 +2479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2419,7 +2493,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
+        <f>1-D9</f>
         <v>0</v>
       </c>
       <c r="F9">
@@ -2444,7 +2518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2458,7 +2532,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="0"/>
+        <f>1-D10</f>
         <v>0</v>
       </c>
       <c r="F10">
@@ -2483,7 +2557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -2497,7 +2571,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
+        <f>1-D11</f>
         <v>1</v>
       </c>
       <c r="F11">
@@ -2536,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="0"/>
+        <f>1-D12</f>
         <v>1</v>
       </c>
       <c r="F12">
@@ -2561,7 +2635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -2575,7 +2649,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="0"/>
+        <f>1-D13</f>
         <v>0</v>
       </c>
       <c r="F13">
@@ -2614,7 +2688,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="0"/>
+        <f>1-D14</f>
         <v>0</v>
       </c>
       <c r="F14">
@@ -2639,7 +2713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2653,7 +2727,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="0"/>
+        <f>1-D15</f>
         <v>0</v>
       </c>
       <c r="F15">
@@ -2679,23 +2753,51 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L15">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L14"/>
+  <sortState ref="A2:L1000">
+    <sortCondition ref="B2:B1000"/>
+  </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2049" r:id="rId3" name="Button 1">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!DateSort">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>12</xdr:col>
+                    <xdr:colOff>419100</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>31750</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>14</xdr:col>
+                    <xdr:colOff>387350</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>95250</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
refine of node_df creation
</commit_message>
<xml_diff>
--- a/Intro.xlsx
+++ b/Intro.xlsx
@@ -8,13 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="sketch" sheetId="1" r:id="rId1"/>
-    <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="data(sample)" sheetId="4" r:id="rId2"/>
     <sheet name="edge_df" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data!$A$1:$L$14</definedName>
-  </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -205,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,6 +221,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -237,11 +240,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -257,10 +261,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1734,77 +1734,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>419100</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>31750</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>14</xdr:col>
-          <xdr:colOff>387350</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2049" name="Button 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2049"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="54864" rIns="36576" bIns="54864" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="游ゴシック"/>
-                  <a:ea typeface="游ゴシック"/>
-                </a:rPr>
-                <a:t>Date ASC</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -2071,9 +2000,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -2152,36 +2079,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="11.08203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.4140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="2"/>
-    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -2207,98 +2128,59 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="A2" s="1">
+        <v>44188</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>IF(D2=0,1,"")</f>
+        <v/>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1">
+        <v>44188</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1">
-        <v>44189</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <f>1-D2</f>
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44190</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
-        <f>1-D3</f>
-        <v>0</v>
+      <c r="E3" s="2" t="str">
+        <f>IF(D3=0,1,"")</f>
+        <v/>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
       <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+      <c r="A4" s="1">
+        <v>44188</v>
+      </c>
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="1">
-        <v>44191</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
       <c r="E4" s="2">
-        <f>1-D4</f>
+        <f>IF(D4=0,1,"")</f>
         <v>1</v>
       </c>
       <c r="F4">
@@ -2307,83 +2189,41 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
       <c r="J4">
         <v>1</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+      <c r="A5" s="1">
+        <v>44192</v>
+      </c>
+      <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="1">
-        <v>44192</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
       <c r="E5" s="2">
-        <f>1-D5</f>
+        <f>IF(D5=0,1,"")</f>
         <v>1</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
       <c r="I5">
         <v>1</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+      <c r="A6" s="1">
+        <v>44193</v>
+      </c>
+      <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="1">
-        <v>44193</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="2">
-        <f>1-D6</f>
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
+      <c r="E6" s="2" t="str">
+        <f>IF(D6=0,1,"")</f>
+        <v/>
       </c>
       <c r="H6">
         <v>1</v>
@@ -2391,404 +2231,199 @@
       <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+      <c r="A7" s="1">
+        <v>44194</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="1">
-        <v>44194</v>
-      </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="2">
-        <f>1-D7</f>
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
+      <c r="E7" s="2" t="str">
+        <f>IF(D7=0,1,"")</f>
+        <v/>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+      <c r="A8" s="1">
+        <v>44195</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="1">
-        <v>44195</v>
-      </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="2">
-        <f>1-D8</f>
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
+      <c r="E8" s="2" t="str">
+        <f>IF(D8=0,1,"")</f>
+        <v/>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
       <c r="L8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+      <c r="A9" s="1">
+        <v>44196</v>
+      </c>
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="1">
-        <v>44196</v>
-      </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="2">
-        <f>1-D9</f>
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
+      <c r="E9" s="2" t="str">
+        <f>IF(D9=0,1,"")</f>
+        <v/>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+      <c r="A10" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1">
-        <v>44197</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" s="2">
-        <f>1-D10</f>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
+      <c r="E10" s="2" t="str">
+        <f>IF(D10=0,1,"")</f>
+        <v/>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+      <c r="A11" s="1">
+        <v>44198</v>
+      </c>
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="1">
-        <v>44198</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
       <c r="E11" s="2">
-        <f>1-D11</f>
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
+        <f>IF(D11=0,1,"")</f>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
       <c r="J11">
         <v>1</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
+      <c r="A12" s="1">
+        <v>44199</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="1">
-        <v>44199</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
       <c r="E12" s="2">
-        <f>1-D12</f>
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
+        <f>IF(D12=0,1,"")</f>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
       <c r="L12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
+      <c r="A13" s="1">
+        <v>44200</v>
+      </c>
+      <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="1">
-        <v>44200</v>
-      </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="2">
-        <f>1-D13</f>
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
+      <c r="E13" s="2" t="str">
+        <f>IF(D13=0,1,"")</f>
+        <v/>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
+      <c r="A14" s="1">
+        <v>44201</v>
+      </c>
+      <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1">
-        <v>44201</v>
-      </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="2">
-        <f>1-D14</f>
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
+      <c r="E14" s="2" t="str">
+        <f>IF(D14=0,1,"")</f>
+        <v/>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
       <c r="L14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
+      <c r="A15" s="1">
+        <v>44202</v>
+      </c>
+      <c r="B15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="1">
-        <v>44202</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="2">
-        <f>1-D15</f>
-        <v>0</v>
+      <c r="E15" s="2" t="str">
+        <f>IF(D15=0,1,"")</f>
+        <v/>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
       <c r="K15">
         <v>1</v>
       </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L14"/>
-  <sortState ref="A2:L1000">
-    <sortCondition ref="B2:B1000"/>
-  </sortState>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2049" r:id="rId3" name="Button 1">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!DateSort">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>12</xdr:col>
-                    <xdr:colOff>419100</xdr:colOff>
-                    <xdr:row>0</xdr:row>
-                    <xdr:rowOff>31750</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>14</xdr:col>
-                    <xdr:colOff>387350</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -2798,7 +2433,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>